<commit_message>
Changed the board for LT parts. Complete redesign with switches.
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
   <si>
     <t>QTY</t>
   </si>
@@ -59,21 +59,6 @@
     <t>Price Point</t>
   </si>
   <si>
-    <t>IC OPAMP GP 700KHZ 8SOIC</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/texas-instruments/LM358DR/296-1014-1-ND/404838</t>
-  </si>
-  <si>
-    <t>296-1014-1-ND</t>
-  </si>
-  <si>
-    <t>LM358DR</t>
-  </si>
-  <si>
-    <t>Inverting Amplification of Signal</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -155,9 +140,6 @@
     <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/PVZ3A103C01B00/490-7102-ND/2603871</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/maxim-integrated/MAX9013ESA-/MAX9013ESA--ND/1495420</t>
-  </si>
-  <si>
     <t>Comparator</t>
   </si>
   <si>
@@ -170,30 +152,15 @@
     <t>Headers</t>
   </si>
   <si>
-    <t>J5,6,7,8</t>
-  </si>
-  <si>
-    <t>R8,18.28.38</t>
-  </si>
-  <si>
     <t>J1,2,3,4</t>
   </si>
   <si>
     <t>Resistor</t>
   </si>
   <si>
-    <t>C1-8</t>
-  </si>
-  <si>
-    <t>U2,4,6,8</t>
-  </si>
-  <si>
     <t>D1-5</t>
   </si>
   <si>
-    <t>U1,3,5,7</t>
-  </si>
-  <si>
     <t>U9</t>
   </si>
   <si>
@@ -221,15 +188,6 @@
     <t>CONSMA001-SMD-G-ND</t>
   </si>
   <si>
-    <t>MAX9013ESA+</t>
-  </si>
-  <si>
-    <t>MAX9013ESA+-ND</t>
-  </si>
-  <si>
-    <t>IC COMP LOW PWR SNGL TTL 8SOIC</t>
-  </si>
-  <si>
     <t>CONN SMA JACK STR 50OHM SMD</t>
   </si>
   <si>
@@ -248,19 +206,94 @@
     <t>952-2264-ND</t>
   </si>
   <si>
-    <t>R2,6,7,12,16,17,22,26,27,32,36,37</t>
-  </si>
-  <si>
-    <t>R1,3,5,11,13,15,21,23,25,31,33,35</t>
-  </si>
-  <si>
-    <t>R4,14,24,34,41</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/texas-instruments/CD4082BM96/296-31523-1-ND/3505803</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>C1-4</t>
+  </si>
+  <si>
+    <t>S1-4</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/c-k-components/JS202011SCQN/401-2002-1-ND/1640098</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE DPDT 300MA 6V</t>
+  </si>
+  <si>
+    <t>JS202011SCQN</t>
+  </si>
+  <si>
+    <t>401-2002-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/linear-technology/LT1809CS6-TRMPBF/LT1809CS6-TRMPBFCT-ND/891475</t>
+  </si>
+  <si>
+    <t>LT1809CS6#TRMPBF</t>
+  </si>
+  <si>
+    <t>LT1809CS6#TRMPBFCT-ND</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 180MHZ RRO TSOT23-6</t>
+  </si>
+  <si>
+    <t>OpAmp</t>
+  </si>
+  <si>
+    <t>A109743CT-ND</t>
+  </si>
+  <si>
+    <t>RLP73K1ER51JTD</t>
+  </si>
+  <si>
+    <t>RES SMD 0.51 OHM 5% 1/8W 0402</t>
+  </si>
+  <si>
+    <t>R5,8,13,18</t>
+  </si>
+  <si>
+    <t>J1,4,6,8</t>
+  </si>
+  <si>
+    <t>U1,4,6,8</t>
+  </si>
+  <si>
+    <t>R4,6,11,16</t>
+  </si>
+  <si>
+    <t>R3,7,12,17,25</t>
+  </si>
+  <si>
+    <t>U2,3,5,7</t>
+  </si>
+  <si>
+    <t>R1,10,15,20</t>
+  </si>
+  <si>
+    <t>R2,9,14,19</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=198213383&amp;uq=635998579766508045</t>
+  </si>
+  <si>
+    <t>LT1719CS8#PBF-ND</t>
+  </si>
+  <si>
+    <t>LT1719CS8#PBF</t>
+  </si>
+  <si>
+    <t>IC COMP R-R I/O SGL 3/5V 8-SOIC</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/linear-technology/LT1719CS8-PBF/LT1719CS8-PBF-ND/889675</t>
   </si>
 </sst>
 </file>
@@ -271,7 +304,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +355,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -356,7 +395,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -382,6 +421,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -667,7 +710,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -719,118 +762,118 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2" s="9">
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I2" s="11">
         <f>G2*F2</f>
-        <v>3.5200000000000002E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F3" s="13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G3" s="9">
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I3" s="11">
-        <f t="shared" ref="I3:I12" si="0">G3*F3</f>
-        <v>4.4400000000000002E-2</v>
+        <f t="shared" ref="I3:I14" si="0">G3*F3</f>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F4" s="13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G4" s="9">
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I4" s="11">
         <f t="shared" si="0"/>
-        <v>4.4400000000000002E-2</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
+        <v>72</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="F5" s="13">
         <v>4</v>
@@ -839,31 +882,31 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I5" s="11">
         <f t="shared" si="0"/>
         <v>1.4079999999999999</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F6" s="8">
         <v>5</v>
@@ -872,31 +915,31 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I6" s="11">
         <f t="shared" si="0"/>
         <v>0.97500000000000009</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F7" s="8">
         <v>5</v>
@@ -905,31 +948,31 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I7" s="11">
         <f t="shared" si="0"/>
         <v>2.35E-2</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2">
         <v>4</v>
@@ -938,31 +981,31 @@
         <v>0.157</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I8" s="11">
         <f t="shared" si="0"/>
         <v>0.628</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2">
         <v>4</v>
@@ -971,64 +1014,64 @@
         <v>3.15</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="I9" s="11">
         <f t="shared" si="0"/>
         <v>12.6</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>64</v>
+        <v>37</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="F10" s="2">
         <v>4</v>
       </c>
       <c r="G10" s="3">
-        <v>2.1800000000000002</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="I10" s="11">
         <f t="shared" si="0"/>
-        <v>8.7200000000000006</v>
+        <v>16.079999999999998</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1037,31 +1080,31 @@
         <v>0.41</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="I11" s="11">
         <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F12" s="2">
         <v>4</v>
@@ -1070,29 +1113,88 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I12" s="11">
         <f t="shared" si="0"/>
         <v>0.29599999999999999</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4</v>
+      </c>
+      <c r="G13" s="19">
+        <v>0.441</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="I13" s="11">
-        <f>SUM(I2:I12)</f>
-        <v>25.1845</v>
+        <f>G13*F13</f>
+        <v>1.764</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="2"/>
-      <c r="I14" s="11"/>
+      <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>9.2899999999999996E-2</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="0"/>
+        <v>0.37159999999999999</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F15" s="2"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5">
+        <f>SUM(I2:I14)</f>
+        <v>34.603299999999997</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I16" s="5"/>
@@ -1107,19 +1209,17 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="J5" r:id="rId1"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J3" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J12" r:id="rId7"/>
-    <hyperlink ref="J8" r:id="rId8"/>
-    <hyperlink ref="J9" r:id="rId9"/>
-    <hyperlink ref="J10" r:id="rId10"/>
-    <hyperlink ref="J11" r:id="rId11"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J4" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="J6" r:id="rId4"/>
+    <hyperlink ref="J7" r:id="rId5"/>
+    <hyperlink ref="J12" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>